<commit_message>
chang folder name + add phase 2
</commit_message>
<xml_diff>
--- a/result_0304.xlsx
+++ b/result_0304.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_data\50_Personal\16_WQIModel\WQi-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF4A349-32FB-4BCD-96D3-1415EEFAB6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAD5DB9-4428-4AFD-8897-0AC17633EFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{67EB1B11-5F84-4CE6-82E6-AD0190963FD3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{67EB1B11-5F84-4CE6-82E6-AD0190963FD3}"/>
   </bookViews>
   <sheets>
     <sheet name="loop200" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="ANN" sheetId="6" r:id="rId4"/>
     <sheet name="Gradient Boosted Tree" sheetId="7" r:id="rId5"/>
     <sheet name="ANN_layers_node" sheetId="9" r:id="rId6"/>
+    <sheet name="Description" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="56">
   <si>
     <t>Set</t>
   </si>
@@ -156,12 +157,66 @@
   <si>
     <t>Number of layers</t>
   </si>
+  <si>
+    <t>Random forest regressor</t>
+  </si>
+  <si>
+    <t>number of decision trees</t>
+  </si>
+  <si>
+    <t>maximum posible dept</t>
+  </si>
+  <si>
+    <t>min samples split</t>
+  </si>
+  <si>
+    <t>min samples leaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Support Vector Regressor </t>
+  </si>
+  <si>
+    <t>kernel</t>
+  </si>
+  <si>
+    <t>radial basic function (rbf)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epsilon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C </t>
+  </si>
+  <si>
+    <t>loss</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activation function </t>
+  </si>
+  <si>
+    <t>Rectified linear unit (ReLU)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optimizer </t>
+  </si>
+  <si>
+    <t>nadam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">learning rate </t>
+  </si>
+  <si>
+    <t>epochs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +258,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -278,7 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -291,6 +352,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -300,7 +364,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1023,56 +1097,56 @@
       </c>
     </row>
     <row r="4" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
-      <c r="P4" s="11" t="s">
+      <c r="P4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
       <c r="U4" s="7"/>
       <c r="V4" s="7"/>
-      <c r="W4" s="11" t="s">
+      <c r="W4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="11"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
       <c r="AB4" s="7"/>
       <c r="AC4" s="7"/>
-      <c r="AD4" s="11" t="s">
+      <c r="AD4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="11"/>
-      <c r="AG4" s="11"/>
-      <c r="AH4" s="11"/>
-      <c r="AK4" s="11" t="s">
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="8"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
+      <c r="AK4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AL4" s="11"/>
-      <c r="AM4" s="11"/>
-      <c r="AN4" s="11"/>
-      <c r="AO4" s="11"/>
+      <c r="AL4" s="8"/>
+      <c r="AM4" s="8"/>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="8"/>
     </row>
     <row r="5" spans="2:41" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
@@ -20742,7 +20816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09AC03B9-55C3-4C7B-B3E4-801C40E7165C}">
   <dimension ref="B3:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U31" sqref="U31"/>
     </sheetView>
   </sheetViews>
@@ -21252,4 +21326,143 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3373EA0E-BBCA-4ED4-9AE3-EB49A1A8482A}">
+  <dimension ref="C5:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C5" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="13">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C6" s="12"/>
+      <c r="D6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C7" s="12"/>
+      <c r="D7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C8" s="12"/>
+      <c r="D8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C10" s="12"/>
+      <c r="D10" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="12"/>
+      <c r="D11" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="12"/>
+      <c r="D13" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="12"/>
+      <c r="D14" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="12"/>
+      <c r="D15" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="13">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="12"/>
+      <c r="D16" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="13">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C12:C16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>